<commit_message>
Multiple sheet import by skipping first sheet
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Downloads\LaraExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D10134E-BB37-4040-A3F2-A635AD828DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2399C28-8615-4ACE-A9C2-5C1469CA5B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="3975" windowWidth="15945" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,15 +36,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>cxv</t>
-  </si>
-  <si>
-    <t>sdfsd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>aksdj</t>
+  </si>
+  <si>
+    <t>sjdf</t>
+  </si>
+  <si>
+    <t>98usdf</t>
+  </si>
+  <si>
+    <t>lksj</t>
+  </si>
+  <si>
+    <t>iu89sd</t>
+  </si>
+  <si>
+    <t>879dfk</t>
+  </si>
+  <si>
+    <t>sdfsdf23</t>
+  </si>
+  <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>xv23r</t>
+  </si>
+  <si>
+    <t>gvdfg</t>
+  </si>
+  <si>
+    <t>sdfgsgs</t>
+  </si>
+  <si>
+    <t>sfsdf</t>
   </si>
 </sst>
 </file>
@@ -360,10 +389,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>3424</v>
+      </c>
+      <c r="B1">
+        <v>23423</v>
+      </c>
+      <c r="C1">
+        <v>24234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>234234</v>
+      </c>
+      <c r="B2">
+        <v>34234</v>
+      </c>
+      <c r="C2">
+        <v>23424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE6F3CD-56C7-4ABD-816E-082120363D20}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,8 +446,55 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F510E98-0288-432B-A01B-D4996AE3F347}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+importing with heading row positioned in different position
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Downloads\LaraExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2399C28-8615-4ACE-A9C2-5C1469CA5B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EC1D7-441B-4B85-A389-2220B378C4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="3975" windowWidth="15945" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="3975" windowWidth="15945" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>aksdj</t>
   </si>
@@ -72,14 +72,31 @@
   </si>
   <si>
     <t>sfsdf</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>award</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,33 +407,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="G5:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="5" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G6">
         <v>3424</v>
       </c>
-      <c r="B1">
+      <c r="J6">
         <v>23423</v>
       </c>
-      <c r="C1">
+      <c r="L6">
         <v>24234</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="7" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G7">
         <v>234234</v>
       </c>
-      <c r="B2">
+      <c r="J7">
         <v>34234</v>
       </c>
-      <c r="C2">
+      <c r="L7">
         <v>23424</v>
       </c>
     </row>
@@ -427,33 +456,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE6F3CD-56C7-4ABD-816E-082120363D20}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -464,33 +504,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F510E98-0288-432B-A01B-D4996AE3F347}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prev commit spreadsheet file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Downloads\LaraExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Downloads\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EC1D7-441B-4B85-A389-2220B378C4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20CF2FB-6513-4A2E-83DF-76A5FC44BCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="3975" windowWidth="15945" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15945" windowHeight="12810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="35">
   <si>
     <t>aksdj</t>
   </si>
@@ -74,13 +74,73 @@
     <t>sfsdf</t>
   </si>
   <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>award</t>
+    <t>Section Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Award / Status</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>csdf</t>
+  </si>
+  <si>
+    <t>f23r</t>
+  </si>
+  <si>
+    <t>no of items</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>vxc</t>
+  </si>
+  <si>
+    <t>dfgdf</t>
+  </si>
+  <si>
+    <t>dhdf</t>
+  </si>
+  <si>
+    <t>cgwer</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>zxc</t>
+  </si>
+  <si>
+    <t>gfhfg</t>
+  </si>
+  <si>
+    <t>gfhf</t>
+  </si>
+  <si>
+    <t>erg</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>vbrt</t>
+  </si>
+  <si>
+    <t>dfrg</t>
+  </si>
+  <si>
+    <t>hgjg</t>
+  </si>
+  <si>
+    <t>age (Year)</t>
+  </si>
+  <si>
+    <t>1dfew</t>
   </si>
 </sst>
 </file>
@@ -112,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,13 +180,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +487,14 @@
   <dimension ref="G5:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G5" s="1" t="s">
@@ -456,15 +537,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE6F3CD-56C7-4ABD-816E-082120363D20}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -475,7 +563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -486,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -495,6 +583,251 @@
       </c>
       <c r="D4" t="s">
         <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -504,15 +837,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F510E98-0288-432B-A01B-D4996AE3F347}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -523,7 +863,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -534,7 +874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -542,6 +882,202 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+if two table are in same heading column
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Downloads\LaraExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAC3E44-2DA9-480C-B2C8-969FF1B8B86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD14DB1-6D00-4A66-AFC4-C088D55590E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15975" yWindow="3540" windowWidth="15945" windowHeight="12810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16035" yWindow="5190" windowWidth="15945" windowHeight="12810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,10 +549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE6F3CD-56C7-4ABD-816E-082120363D20}">
-  <dimension ref="B2:K23"/>
+  <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,12 +560,13 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -576,7 +577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -586,14 +587,8 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -612,14 +607,8 @@
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="2">
-        <v>34928</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -639,7 +628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -659,7 +648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -673,7 +662,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -687,7 +676,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -701,7 +690,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -712,7 +701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -722,8 +711,14 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -733,8 +728,14 @@
       <c r="D12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="2">
+        <v>34928</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -745,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -756,7 +757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -767,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -857,15 +858,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F510E98-0288-432B-A01B-D4996AE3F347}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,12 +875,13 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -889,7 +892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -899,14 +902,8 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -925,14 +922,8 @@
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -952,7 +943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -972,7 +963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -992,7 +983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +997,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1020,7 +1011,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1041,8 +1032,14 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1052,8 +1049,14 @@
       <c r="D12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="2">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
+marging columns & hinding columns on same row position
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Downloads\LaraExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD14DB1-6D00-4A66-AFC4-C088D55590E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897A0ADC-F290-4E2D-9C8A-B432BC592BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16035" yWindow="5190" windowWidth="15945" windowHeight="12810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12120" yWindow="2640" windowWidth="15945" windowHeight="12810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="45">
   <si>
     <t>aksdj</t>
   </si>
@@ -95,21 +95,6 @@
     <t>no of items</t>
   </si>
   <si>
-    <t>sdfsd</t>
-  </si>
-  <si>
-    <t>vxc</t>
-  </si>
-  <si>
-    <t>dfgdf</t>
-  </si>
-  <si>
-    <t>dhdf</t>
-  </si>
-  <si>
-    <t>cgwer</t>
-  </si>
-  <si>
     <t>asdas</t>
   </si>
   <si>
@@ -140,9 +125,6 @@
     <t>age (Year)</t>
   </si>
   <si>
-    <t>1dfew</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -153,13 +135,49 @@
   </si>
   <si>
     <t>any heading</t>
+  </si>
+  <si>
+    <t>asdx</t>
+  </si>
+  <si>
+    <t>xcvr</t>
+  </si>
+  <si>
+    <t>dfgdg</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>qasd</t>
+  </si>
+  <si>
+    <t>vrw</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>James Smith</t>
+  </si>
+  <si>
+    <t>Sam Smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +189,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,11 +235,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +580,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE6F3CD-56C7-4ABD-816E-082120363D20}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,13 +591,14 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -577,7 +609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -588,7 +620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -598,17 +630,21 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4">
+        <v>123</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -618,17 +654,21 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5">
+        <v>222</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -638,17 +678,21 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6">
+        <v>333</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -658,11 +702,21 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7">
+        <v>444</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -672,11 +726,15 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8">
+        <v>555</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -686,11 +744,12 @@
       <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -701,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -711,14 +770,14 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -728,14 +787,14 @@
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="2">
         <v>34928</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -746,7 +805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -757,7 +816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -767,8 +826,15 @@
       <c r="D15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -778,8 +844,15 @@
       <c r="D16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -789,8 +862,14 @@
       <c r="D17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -801,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -812,7 +891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -823,7 +902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -834,7 +913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -845,7 +924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -857,6 +936,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -864,10 +951,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F510E98-0288-432B-A01B-D4996AE3F347}">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,13 +962,14 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -892,7 +980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -903,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -913,17 +1001,21 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4">
+        <v>123</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -933,17 +1025,21 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5">
+        <v>643</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -953,17 +1049,21 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6">
+        <v>532</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -973,17 +1073,21 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7">
+        <v>316</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -993,11 +1097,15 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8">
+        <v>424</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1007,11 +1115,15 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9">
+        <v>854</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1022,7 +1134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1032,14 +1144,14 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1049,14 +1161,14 @@
       <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="2">
         <v>928</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -1067,7 +1179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -1078,7 +1190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -1088,8 +1200,15 @@
       <c r="D15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -1099,8 +1218,14 @@
       <c r="D16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1110,8 +1235,15 @@
       <c r="D17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -1123,6 +1255,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>